<commit_message>
Finish creating all data
</commit_message>
<xml_diff>
--- a/data/nurse.xlsx
+++ b/data/nurse.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://merced-my.sharepoint.com/personal/ypalaciosguzman_ucmerced_edu/Documents/Fall21/Hospital_Management_System/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="11_F25DC773A252ABDACC10480A791A596E5ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F31F09C8-A625-4512-9913-42255FE02473}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="11_F25DC773A252ABDACC10480A791A596E5ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A73F70B6-91A8-4C09-926A-707FF67AEAFD}"/>
   <bookViews>
-    <workbookView xWindow="45765" yWindow="1590" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3780" yWindow="1920" windowWidth="20130" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,23 +34,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="74">
   <si>
     <t>name</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
     <t>started_working</t>
   </si>
   <si>
     <t>phone_number</t>
   </si>
   <si>
-    <t>hospital_id</t>
-  </si>
-  <si>
     <t>4f205924-80dc-4cb3-a6d1-e13bbbdd716a</t>
   </si>
   <si>
@@ -196,13 +190,79 @@
   </si>
   <si>
     <t>Lily Wyatt</t>
+  </si>
+  <si>
+    <t>n_id</t>
+  </si>
+  <si>
+    <t>h_id</t>
+  </si>
+  <si>
+    <t>Ezequiel</t>
+  </si>
+  <si>
+    <t>Isaias</t>
+  </si>
+  <si>
+    <t>Issac</t>
+  </si>
+  <si>
+    <t>Jaiden</t>
+  </si>
+  <si>
+    <t>Jasiah</t>
+  </si>
+  <si>
+    <t>Joziah</t>
+  </si>
+  <si>
+    <t>Julien</t>
+  </si>
+  <si>
+    <t>Kaiden</t>
+  </si>
+  <si>
+    <t>Kairo</t>
+  </si>
+  <si>
+    <t>Kaison</t>
+  </si>
+  <si>
+    <t>Kalel</t>
+  </si>
+  <si>
+    <t>Kameron</t>
+  </si>
+  <si>
+    <t>Kamryn</t>
+  </si>
+  <si>
+    <t>Juelz</t>
+  </si>
+  <si>
+    <t>Jovanni</t>
+  </si>
+  <si>
+    <t>Johnathan</t>
+  </si>
+  <si>
+    <t>Jeffery</t>
+  </si>
+  <si>
+    <t>Jakob</t>
+  </si>
+  <si>
+    <t>Jaime</t>
+  </si>
+  <si>
+    <t>Izaiah</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -214,6 +274,11 @@
       <sz val="11"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -236,12 +301,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -523,10 +591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,29 +606,32 @@
     <col min="5" max="5" width="37.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
       <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1">
         <v>44011</v>
@@ -569,15 +640,18 @@
         <v>7680480133</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1">
         <v>42658</v>
@@ -586,15 +660,18 @@
         <v>9481722088</v>
       </c>
       <c r="E3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C4" s="1">
         <v>42381</v>
@@ -603,15 +680,18 @@
         <v>9690161816</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C5" s="1">
         <v>43729</v>
@@ -620,15 +700,18 @@
         <v>6197080058</v>
       </c>
       <c r="E5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C6" s="1">
         <v>41253</v>
@@ -637,15 +720,18 @@
         <v>9690834495</v>
       </c>
       <c r="E6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C7" s="1">
         <v>41534</v>
@@ -654,15 +740,18 @@
         <v>8436894894</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C8" s="1">
         <v>43114</v>
@@ -671,15 +760,18 @@
         <v>8096295277</v>
       </c>
       <c r="E8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C9" s="1">
         <v>39166</v>
@@ -688,15 +780,18 @@
         <v>6262096706</v>
       </c>
       <c r="E9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C10" s="1">
         <v>38088</v>
@@ -705,15 +800,18 @@
         <v>6256857943</v>
       </c>
       <c r="E10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C11" s="1">
         <v>38354</v>
@@ -722,15 +820,18 @@
         <v>9263007051</v>
       </c>
       <c r="E11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C12" s="1">
         <v>40661</v>
@@ -739,15 +840,18 @@
         <v>7925848392</v>
       </c>
       <c r="E12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C13" s="1">
         <v>38863</v>
@@ -756,15 +860,18 @@
         <v>9264726531</v>
       </c>
       <c r="E13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C14" s="1">
         <v>43692</v>
@@ -773,15 +880,18 @@
         <v>8582353377</v>
       </c>
       <c r="E14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C15" s="1">
         <v>39067</v>
@@ -790,15 +900,18 @@
         <v>6826554768</v>
       </c>
       <c r="E15" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C16" s="1">
         <v>36969</v>
@@ -807,15 +920,18 @@
         <v>6062973937</v>
       </c>
       <c r="E16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C17" s="1">
         <v>40863</v>
@@ -824,15 +940,18 @@
         <v>7381427843</v>
       </c>
       <c r="E17" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C18" s="1">
         <v>40438</v>
@@ -841,15 +960,18 @@
         <v>8905752540</v>
       </c>
       <c r="E18" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C19" s="1">
         <v>38196</v>
@@ -858,15 +980,18 @@
         <v>6123011230</v>
       </c>
       <c r="E19" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B20" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C20" s="1">
         <v>39111</v>
@@ -875,15 +1000,18 @@
         <v>7731946055</v>
       </c>
       <c r="E20" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B21" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C21" s="1">
         <v>42779</v>
@@ -892,7 +1020,10 @@
         <v>8942113164</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>